<commit_message>
CRUD for Prospectus Version, Courses, View Student Info 50%
</commit_message>
<xml_diff>
--- a/public/excel/ImportSubjects.xlsx
+++ b/public/excel/ImportSubjects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\AcademicPreEnlistmentSystem\public\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHRIS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Description</t>
   </si>
@@ -330,35 +330,27 @@
     <t>Semester</t>
   </si>
   <si>
-    <t>Course</t>
-  </si>
-  <si>
-    <t>Bachelor of Science in Information Technology</t>
-  </si>
-  <si>
-    <t>CourseAbbreviation</t>
-  </si>
-  <si>
-    <t>BSIT</t>
-  </si>
-  <si>
-    <t>CMO No 25, S.2015, BOR No. 18, S. 2018</t>
-  </si>
-  <si>
-    <t>S.Y. 2023-2024</t>
-  </si>
-  <si>
-    <t>ProspectusVersion</t>
-  </si>
-  <si>
-    <t>ProspectusEffectivityDate</t>
+    <t>IT Elective 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>None</t>
+    </r>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +360,23 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -392,9 +401,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +726,7 @@
     <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -718,20 +748,8 @@
       <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -753,20 +771,8 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -789,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -812,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -835,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -858,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -881,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -904,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -927,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -950,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -973,7 +979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -996,7 +1002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1154,6 +1160,52 @@
         <v>1</v>
       </c>
       <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="6">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8">
+        <v>3</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
+        <v>2</v>
+      </c>
+      <c r="G21" s="8">
         <v>2</v>
       </c>
     </row>

</xml_diff>